<commit_message>
1.Developed a new test in catalog module - VerifyReq_CopyItemsForRFQCancelledStatus. 2. Added a new method in CartInformationPage - verifyAddedCartItem_ForRejectedOrder. 3. Added a new method in ItemDetailsPage - addCopiedItemToCart_RejectedOrders. 4. Added a new method in RequisitioningPage - copyRFQCancelledItem.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyReq_CopyRFQCancelledItems.xlsx
+++ b/src/test/resources/datasheets/VerifyReq_CopyRFQCancelledItems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="14220" windowHeight="3015"/>
   </bookViews>
   <sheets>
     <sheet name="CopyRFQCancelledItems" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Role</t>
   </si>
@@ -28,6 +29,18 @@
   </si>
   <si>
     <t xml:space="preserve">Location                      </t>
+  </si>
+  <si>
+    <t>unitPrice</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>UOMValue</t>
+  </si>
+  <si>
+    <t>CU-CUBIC</t>
   </si>
 </sst>
 </file>
@@ -359,31 +372,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>